<commit_message>
update parameters for API
</commit_message>
<xml_diff>
--- a/Documentation/Design plan/In_output_parameters.xlsx
+++ b/Documentation/Design plan/In_output_parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasper\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasper\Documents\TU Delft\Bsc3\Minor\Computer Science Project\ewi3615tu-ds7\Documentation\Design plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4424AFEE-74DA-4B85-AF78-0691C7D8CDC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C128B286-56F3-488E-81A0-2A55EC66489A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{E361D52F-B2A5-4CFC-A55B-E0A38AABCDAD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>inputs</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>list of segment information</t>
-  </si>
-  <si>
-    <t>number of entries for leaderboard</t>
   </si>
   <si>
     <t>Module</t>
@@ -128,12 +125,29 @@
 coordinates of segments</t>
   </si>
   <si>
-    <t>list of segment IDs
-list of segment coordinates</t>
-  </si>
-  <si>
     <t>number of entries for leaderboard
 all entries</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>/segments/explore</t>
+  </si>
+  <si>
+    <t>list of segment IDs
+list of segment coordinates
+segment length in m</t>
+  </si>
+  <si>
+    <t>/segments/{id}/leaderboard</t>
+  </si>
+  <si>
+    <t>number of entries for segment</t>
+  </si>
+  <si>
+    <t>compare elapsed time with segment length to compute  velocity, use minimum velocity theshold 
+optional: use statistics to identify outliers (check distribution type!)</t>
   </si>
 </sst>
 </file>
@@ -491,145 +505,166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6778F579-1AA2-4935-86A2-3471B07B087C}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="102" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="16.83984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.7890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.578125" customWidth="1"/>
     <col min="4" max="4" width="54.3125" customWidth="1"/>
+    <col min="5" max="5" width="27.734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" s="1"/>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="1"/>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added PackageInterfaces diagram, Closes #3
</commit_message>
<xml_diff>
--- a/Documentation/Design plan/In_output_parameters.xlsx
+++ b/Documentation/Design plan/In_output_parameters.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasper\Documents\TU Delft\Bsc3\Minor\Computer Science Project\ewi3615tu-ds7\Documentation\Design plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\lmaio\Nextcloud\TU Delft\2019-2020\CS Project\ewi3615tu-ds7\Documentation\Design plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C128B286-56F3-488E-81A0-2A55EC66489A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{E361D52F-B2A5-4CFC-A55B-E0A38AABCDAD}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="15450" windowHeight="8430"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -100,9 +99,6 @@
 date range</t>
   </si>
   <si>
-    <t>Heat map</t>
-  </si>
-  <si>
     <t>number of entries for leaderboard
 all entries
 minimum velocity?
@@ -117,10 +113,6 @@
 time-of-day</t>
   </si>
   <si>
-    <t>segment coordinates
-segment entries</t>
-  </si>
-  <si>
     <t>number of entries for leaderboard for all segments per time of day
 coordinates of segments</t>
   </si>
@@ -148,12 +140,20 @@
   <si>
     <t>compare elapsed time with segment length to compute  velocity, use minimum velocity theshold 
 optional: use statistics to identify outliers (check distribution type!)</t>
+  </si>
+  <si>
+    <t>segment coordinates
+segment entries
+location</t>
+  </si>
+  <si>
+    <t>Heat map (HTML webpage)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -504,23 +504,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6778F579-1AA2-4935-86A2-3471B07B087C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="102" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="102" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.578125" customWidth="1"/>
-    <col min="4" max="4" width="54.3125" customWidth="1"/>
-    <col min="5" max="5" width="27.734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="54.28515625" customWidth="1"/>
+    <col min="5" max="5" width="65.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -528,7 +529,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -537,7 +538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -547,16 +548,16 @@
         <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>18</v>
@@ -565,7 +566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
@@ -575,59 +576,59 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
@@ -635,7 +636,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
@@ -643,7 +644,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -654,17 +655,17 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update output of strava module
</commit_message>
<xml_diff>
--- a/Documentation/Design plan/In_output_parameters.xlsx
+++ b/Documentation/Design plan/In_output_parameters.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\lmaio\Nextcloud\TU Delft\2019-2020\CS Project\ewi3615tu-ds7\Documentation\Design plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasper\Documents\TU Delft\Bsc3\Minor\Computer Science Project\ewi3615tu-ds7\Documentation\Design plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4953A14-2B60-473F-88BB-A5138AABE77D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="15450" windowHeight="8430"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -113,10 +108,6 @@
 time-of-day</t>
   </si>
   <si>
-    <t>number of entries for leaderboard for all segments per time of day
-coordinates of segments</t>
-  </si>
-  <si>
     <t>number of entries for leaderboard
 all entries</t>
   </si>
@@ -148,12 +139,17 @@
   </si>
   <si>
     <t>Heat map (HTML webpage)</t>
+  </si>
+  <si>
+    <t>number of entries for leaderboard for all segments per time of day
+coordinates of segments
+date range</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -504,24 +500,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="102" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="54.28515625" customWidth="1"/>
-    <col min="5" max="5" width="65.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.68359375" customWidth="1"/>
+    <col min="3" max="3" width="43.578125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="54.26171875" customWidth="1"/>
+    <col min="5" max="5" width="65.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -529,7 +525,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -538,7 +534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -548,16 +544,16 @@
         <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>18</v>
@@ -566,7 +562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
@@ -576,40 +572,40 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -618,7 +614,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
@@ -628,7 +624,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
@@ -636,7 +632,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
@@ -644,7 +640,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -655,17 +651,17 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>